<commit_message>
ship: fixes in bulk
</commit_message>
<xml_diff>
--- a/import/CCYYYYcreator@dariah.eu.xlsx
+++ b/import/CCYYYYcreator@dariah.eu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dirk/github/Dans-labs/dariah-contrib/import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC7FDE4-4E6C-F54C-97B7-2F7DAA66AB6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6068F8-B8BE-D242-9028-5FB05699AE9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28600" windowHeight="20540" xr2:uid="{9E4E58A0-E663-B14C-8CE3-230EC566B6AD}"/>
   </bookViews>
@@ -1627,7 +1627,8 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> must be filled with a number, without a decimal point and without thousand-separators, and without a currency indicator. The amount is taken in € (euros).
-Copy this template to a file with a name that contains the country, the year and your email address as specified below. That information will be extracted and used for the contributions when they are imported into the system.
+Copy this template to a file with a name that contains the country, the year and your EPPN as specified below. That information will be extracted and used for the contributions when they are imported into the system.
+Your EPPN is visible on the interface when you are logged in: click the triangle in front of your name in the top right corner.
 </t>
     </r>
   </si>
@@ -1707,10 +1708,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2044,11 +2045,11 @@
       <c r="A1" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>506</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" ht="17">
       <c r="A2" s="3" t="s">
@@ -2932,12 +2933,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="14">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Unknown value" error="Allowed values are listed in the corresponding sheet._x000a_" xr:uid="{1BC46876-2CF4-4040-AA4F-6C62FA310533}">
           <x14:formula1>
             <xm:f>typeContribution!$A$1:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B129</xm:sqref>
+          <xm:sqref>B2:B129</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unknown value" error="Allowed values are listed in the corresponding sheet._x000a_" xr:uid="{A2274C7F-382B-DA4E-BA2D-99F2D43A77D1}">
           <x14:formula1>
@@ -2980,12 +2981,6 @@
             <xm:f>tadirahObject!$A$1:$A$36</xm:f>
           </x14:formula1>
           <xm:sqref>K2:K128</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Unknown value" error="Allowed values are listed in the corresponding sheet._x000a_" xr:uid="{7008AF30-165E-6041-8A7E-9EAE48E953A0}">
-          <x14:formula1>
-            <xm:f>typeContribution!$A$1:$A$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B128</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Unknown value" error="Allowed values are listed in the corresponding sheet._x000a_" xr:uid="{8C924306-AB8B-B44B-A98B-608EAECD09B9}">
           <x14:formula1>
@@ -3348,7 +3343,7 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="C45" s="9"/>
+      <c r="C45" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>